<commit_message>
trmnt flight start from id 100
</commit_message>
<xml_diff>
--- a/src/excel_downloads/Mock Schedule and Results for Swap 3-9-2020.xlsx
+++ b/src/excel_downloads/Mock Schedule and Results for Swap 3-9-2020.xlsx
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="K2" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
         </is>
       </c>
       <c r="K3" t="n">
-        <v>879</v>
+        <v>101</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="K4" t="n">
-        <v>880</v>
+        <v>102</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="K5" t="n">
-        <v>881</v>
+        <v>103</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -758,7 +758,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>882</v>
+        <v>104</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="K7" t="n">
-        <v>883</v>
+        <v>105</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="K8" t="n">
-        <v>884</v>
+        <v>106</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="K9" t="n">
-        <v>885</v>
+        <v>107</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>886</v>
+        <v>108</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="K11" t="n">
-        <v>887</v>
+        <v>109</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
@@ -1150,7 +1150,7 @@
         </is>
       </c>
       <c r="K12" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
@@ -1216,7 +1216,7 @@
         </is>
       </c>
       <c r="K13" t="n">
-        <v>888</v>
+        <v>110</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1284,7 +1284,7 @@
         </is>
       </c>
       <c r="K14" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
@@ -1348,7 +1348,7 @@
         </is>
       </c>
       <c r="K15" t="n">
-        <v>889</v>
+        <v>111</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="K16" t="n">
-        <v>890</v>
+        <v>112</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1476,7 +1476,7 @@
         </is>
       </c>
       <c r="K17" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1544,7 +1544,7 @@
         </is>
       </c>
       <c r="K18" t="n">
-        <v>891</v>
+        <v>114</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
@@ -1608,7 +1608,7 @@
         </is>
       </c>
       <c r="K19" t="n">
-        <v>892</v>
+        <v>115</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1668,7 +1668,7 @@
         </is>
       </c>
       <c r="K20" t="n">
-        <v>893</v>
+        <v>116</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
@@ -1796,7 +1796,7 @@
         </is>
       </c>
       <c r="K22" t="n">
-        <v>894</v>
+        <v>117</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="K23" t="n">
-        <v>895</v>
+        <v>118</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
@@ -1928,7 +1928,7 @@
         </is>
       </c>
       <c r="K24" t="n">
-        <v>896</v>
+        <v>119</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="K25" t="n">
-        <v>897</v>
+        <v>120</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -2060,7 +2060,7 @@
         </is>
       </c>
       <c r="K26" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
@@ -2124,7 +2124,7 @@
         </is>
       </c>
       <c r="K27" t="n">
-        <v>898</v>
+        <v>121</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="K28" t="n">
-        <v>899</v>
+        <v>122</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
@@ -2258,7 +2258,7 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -2318,7 +2318,7 @@
         </is>
       </c>
       <c r="K30" t="n">
-        <v>900</v>
+        <v>123</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -2388,7 +2388,7 @@
         </is>
       </c>
       <c r="K31" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="K32" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
@@ -2520,7 +2520,7 @@
         </is>
       </c>
       <c r="K33" t="n">
-        <v>901</v>
+        <v>125</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
@@ -2584,7 +2584,7 @@
         </is>
       </c>
       <c r="K34" t="n">
-        <v>902</v>
+        <v>126</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2648,7 +2648,7 @@
         </is>
       </c>
       <c r="K35" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
@@ -2708,7 +2708,7 @@
         </is>
       </c>
       <c r="K36" t="n">
-        <v>903</v>
+        <v>127</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
@@ -2776,7 +2776,7 @@
         </is>
       </c>
       <c r="K37" t="n">
-        <v>904</v>
+        <v>128</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2840,7 +2840,7 @@
         </is>
       </c>
       <c r="K38" t="n">
-        <v>905</v>
+        <v>129</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2908,7 +2908,7 @@
         </is>
       </c>
       <c r="K39" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
@@ -2978,7 +2978,7 @@
         </is>
       </c>
       <c r="K40" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
@@ -3044,7 +3044,7 @@
         </is>
       </c>
       <c r="K41" t="n">
-        <v>906</v>
+        <v>130</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
@@ -3112,7 +3112,7 @@
         </is>
       </c>
       <c r="K42" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
@@ -3172,7 +3172,7 @@
         </is>
       </c>
       <c r="K43" t="n">
-        <v>907</v>
+        <v>131</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -3242,7 +3242,7 @@
         </is>
       </c>
       <c r="K44" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
@@ -3306,7 +3306,7 @@
         </is>
       </c>
       <c r="K45" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -3374,7 +3374,7 @@
         </is>
       </c>
       <c r="K46" t="n">
-        <v>908</v>
+        <v>132</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -3438,7 +3438,7 @@
         </is>
       </c>
       <c r="K47" t="n">
-        <v>909</v>
+        <v>133</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
@@ -3498,7 +3498,7 @@
         </is>
       </c>
       <c r="K48" t="n">
-        <v>910</v>
+        <v>134</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -3562,7 +3562,7 @@
         </is>
       </c>
       <c r="K49" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="K50" t="n">
-        <v>911</v>
+        <v>135</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -3690,7 +3690,7 @@
         </is>
       </c>
       <c r="K51" t="n">
-        <v>912</v>
+        <v>136</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -3754,7 +3754,7 @@
         </is>
       </c>
       <c r="K52" t="n">
-        <v>913</v>
+        <v>137</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="K53" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
@@ -3886,7 +3886,7 @@
         </is>
       </c>
       <c r="K54" t="n">
-        <v>914</v>
+        <v>138</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -3956,7 +3956,7 @@
         </is>
       </c>
       <c r="K55" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
@@ -4022,7 +4022,7 @@
         </is>
       </c>
       <c r="K56" t="n">
-        <v>915</v>
+        <v>139</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
@@ -4090,7 +4090,7 @@
         </is>
       </c>
       <c r="K57" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
@@ -4150,7 +4150,7 @@
         </is>
       </c>
       <c r="K58" t="n">
-        <v>916</v>
+        <v>140</v>
       </c>
       <c r="L58" t="inlineStr">
         <is>
@@ -4220,7 +4220,7 @@
         </is>
       </c>
       <c r="K59" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L59" t="inlineStr">
         <is>
@@ -4284,7 +4284,7 @@
         </is>
       </c>
       <c r="K60" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L60" t="inlineStr">
         <is>
@@ -4352,7 +4352,7 @@
         </is>
       </c>
       <c r="K61" t="n">
-        <v>917</v>
+        <v>141</v>
       </c>
       <c r="L61" t="inlineStr">
         <is>
@@ -4416,7 +4416,7 @@
         </is>
       </c>
       <c r="K62" t="n">
-        <v>918</v>
+        <v>142</v>
       </c>
       <c r="L62" t="inlineStr">
         <is>
@@ -4476,7 +4476,7 @@
         </is>
       </c>
       <c r="K63" t="n">
-        <v>919</v>
+        <v>143</v>
       </c>
       <c r="L63" t="inlineStr">
         <is>
@@ -4540,7 +4540,7 @@
         </is>
       </c>
       <c r="K64" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L64" t="inlineStr">
         <is>
@@ -4600,7 +4600,7 @@
         </is>
       </c>
       <c r="K65" t="n">
-        <v>920</v>
+        <v>144</v>
       </c>
       <c r="L65" t="inlineStr">
         <is>
@@ -4668,7 +4668,7 @@
         </is>
       </c>
       <c r="K66" t="n">
-        <v>921</v>
+        <v>145</v>
       </c>
       <c r="L66" t="inlineStr">
         <is>
@@ -4732,7 +4732,7 @@
         </is>
       </c>
       <c r="K67" t="n">
-        <v>922</v>
+        <v>146</v>
       </c>
       <c r="L67" t="inlineStr">
         <is>
@@ -4800,7 +4800,7 @@
         </is>
       </c>
       <c r="K68" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L68" t="inlineStr">
         <is>
@@ -4870,7 +4870,7 @@
         </is>
       </c>
       <c r="K69" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L69" t="inlineStr">
         <is>
@@ -4936,7 +4936,7 @@
         </is>
       </c>
       <c r="K70" t="n">
-        <v>923</v>
+        <v>147</v>
       </c>
       <c r="L70" t="inlineStr">
         <is>
@@ -5006,7 +5006,7 @@
         </is>
       </c>
       <c r="K71" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L71" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
         </is>
       </c>
       <c r="K72" t="n">
-        <v>924</v>
+        <v>148</v>
       </c>
       <c r="L72" t="inlineStr">
         <is>
@@ -5130,7 +5130,7 @@
         </is>
       </c>
       <c r="K73" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L73" t="inlineStr">
         <is>
@@ -5198,7 +5198,7 @@
         </is>
       </c>
       <c r="K74" t="n">
-        <v>925</v>
+        <v>149</v>
       </c>
       <c r="L74" t="inlineStr">
         <is>
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="K75" t="n">
-        <v>926</v>
+        <v>150</v>
       </c>
       <c r="L75" t="inlineStr">
         <is>
@@ -5334,7 +5334,7 @@
         </is>
       </c>
       <c r="K76" t="n">
-        <v>570</v>
+        <v>100</v>
       </c>
       <c r="L76" t="inlineStr">
         <is>
@@ -5394,7 +5394,7 @@
         </is>
       </c>
       <c r="K77" t="n">
-        <v>927</v>
+        <v>151</v>
       </c>
       <c r="L77" t="inlineStr">
         <is>
@@ -5458,7 +5458,7 @@
         </is>
       </c>
       <c r="K78" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L78" t="inlineStr">
         <is>
@@ -5522,7 +5522,7 @@
         </is>
       </c>
       <c r="K79" t="n">
-        <v>928</v>
+        <v>152</v>
       </c>
       <c r="L79" t="inlineStr">
         <is>
@@ -5586,7 +5586,7 @@
         </is>
       </c>
       <c r="K80" t="n">
-        <v>929</v>
+        <v>153</v>
       </c>
       <c r="L80" t="inlineStr">
         <is>
@@ -5650,7 +5650,7 @@
         </is>
       </c>
       <c r="K81" t="n">
-        <v>930</v>
+        <v>154</v>
       </c>
       <c r="L81" t="inlineStr">
         <is>
@@ -5720,7 +5720,7 @@
         </is>
       </c>
       <c r="K82" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L82" t="inlineStr">
         <is>
@@ -5786,7 +5786,7 @@
         </is>
       </c>
       <c r="K83" t="n">
-        <v>931</v>
+        <v>155</v>
       </c>
       <c r="L83" t="inlineStr">
         <is>
@@ -5850,7 +5850,7 @@
         </is>
       </c>
       <c r="K84" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L84" t="inlineStr">
         <is>
@@ -5918,7 +5918,7 @@
         </is>
       </c>
       <c r="K85" t="n">
-        <v>932</v>
+        <v>157</v>
       </c>
       <c r="L85" t="inlineStr">
         <is>
@@ -5992,7 +5992,7 @@
         </is>
       </c>
       <c r="K86" t="n">
-        <v>569</v>
+        <v>124</v>
       </c>
       <c r="L86" t="inlineStr">
         <is>
@@ -6056,7 +6056,7 @@
         </is>
       </c>
       <c r="K87" t="n">
-        <v>933</v>
+        <v>158</v>
       </c>
       <c r="L87" t="inlineStr">
         <is>
@@ -6124,7 +6124,7 @@
         </is>
       </c>
       <c r="K88" t="n">
-        <v>583</v>
+        <v>113</v>
       </c>
       <c r="L88" t="inlineStr">
         <is>
@@ -6184,7 +6184,7 @@
         </is>
       </c>
       <c r="K89" t="n">
-        <v>934</v>
+        <v>159</v>
       </c>
       <c r="L89" t="inlineStr">
         <is>
@@ -6252,7 +6252,7 @@
         </is>
       </c>
       <c r="K90" t="n">
-        <v>935</v>
+        <v>160</v>
       </c>
       <c r="L90" t="inlineStr">
         <is>
@@ -6316,7 +6316,7 @@
         </is>
       </c>
       <c r="K91" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L91" t="inlineStr">
         <is>
@@ -6384,7 +6384,7 @@
         </is>
       </c>
       <c r="K92" t="n">
-        <v>936</v>
+        <v>161</v>
       </c>
       <c r="L92" t="inlineStr">
         <is>
@@ -6450,7 +6450,7 @@
         </is>
       </c>
       <c r="K93" t="n">
-        <v>937</v>
+        <v>162</v>
       </c>
       <c r="L93" t="inlineStr">
         <is>
@@ -6514,7 +6514,7 @@
         </is>
       </c>
       <c r="K94" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L94" t="inlineStr">
         <is>
@@ -6584,7 +6584,7 @@
         </is>
       </c>
       <c r="K95" t="n">
-        <v>938</v>
+        <v>163</v>
       </c>
       <c r="L95" t="inlineStr">
         <is>
@@ -6652,7 +6652,7 @@
         </is>
       </c>
       <c r="K96" t="n">
-        <v>939</v>
+        <v>164</v>
       </c>
       <c r="L96" t="inlineStr">
         <is>
@@ -6716,7 +6716,7 @@
         </is>
       </c>
       <c r="K97" t="n">
-        <v>940</v>
+        <v>165</v>
       </c>
       <c r="L97" t="inlineStr">
         <is>
@@ -6776,7 +6776,7 @@
         </is>
       </c>
       <c r="K98" t="n">
-        <v>941</v>
+        <v>166</v>
       </c>
       <c r="L98" t="inlineStr">
         <is>
@@ -6840,7 +6840,7 @@
         </is>
       </c>
       <c r="K99" t="n">
-        <v>942</v>
+        <v>167</v>
       </c>
       <c r="L99" t="inlineStr">
         <is>
@@ -6904,7 +6904,7 @@
         </is>
       </c>
       <c r="K100" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L100" t="inlineStr">
         <is>
@@ -6972,7 +6972,7 @@
         </is>
       </c>
       <c r="K101" t="n">
-        <v>943</v>
+        <v>168</v>
       </c>
       <c r="L101" t="inlineStr">
         <is>
@@ -7040,7 +7040,7 @@
         </is>
       </c>
       <c r="K102" t="n">
-        <v>944</v>
+        <v>169</v>
       </c>
       <c r="L102" t="inlineStr">
         <is>
@@ -7104,7 +7104,7 @@
         </is>
       </c>
       <c r="K103" t="n">
-        <v>945</v>
+        <v>170</v>
       </c>
       <c r="L103" t="inlineStr">
         <is>
@@ -7170,7 +7170,7 @@
         </is>
       </c>
       <c r="K104" t="n">
-        <v>946</v>
+        <v>171</v>
       </c>
       <c r="L104" t="inlineStr">
         <is>
@@ -7234,7 +7234,7 @@
         </is>
       </c>
       <c r="K105" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L105" t="inlineStr">
         <is>
@@ -7302,7 +7302,7 @@
         </is>
       </c>
       <c r="K106" t="n">
-        <v>947</v>
+        <v>172</v>
       </c>
       <c r="L106" t="inlineStr">
         <is>
@@ -7370,7 +7370,7 @@
         </is>
       </c>
       <c r="K107" t="n">
-        <v>948</v>
+        <v>173</v>
       </c>
       <c r="L107" t="inlineStr">
         <is>
@@ -7434,7 +7434,7 @@
         </is>
       </c>
       <c r="K108" t="n">
-        <v>949</v>
+        <v>174</v>
       </c>
       <c r="L108" t="inlineStr">
         <is>
@@ -7494,7 +7494,7 @@
         </is>
       </c>
       <c r="K109" t="n">
-        <v>950</v>
+        <v>175</v>
       </c>
       <c r="L109" t="inlineStr">
         <is>
@@ -7558,7 +7558,7 @@
         </is>
       </c>
       <c r="K110" t="n">
-        <v>951</v>
+        <v>176</v>
       </c>
       <c r="L110" t="inlineStr">
         <is>
@@ -7622,7 +7622,7 @@
         </is>
       </c>
       <c r="K111" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L111" t="inlineStr">
         <is>
@@ -7690,7 +7690,7 @@
         </is>
       </c>
       <c r="K112" t="n">
-        <v>952</v>
+        <v>177</v>
       </c>
       <c r="L112" t="inlineStr">
         <is>
@@ -7760,7 +7760,7 @@
         </is>
       </c>
       <c r="K113" t="n">
-        <v>953</v>
+        <v>178</v>
       </c>
       <c r="L113" t="inlineStr">
         <is>
@@ -7824,7 +7824,7 @@
         </is>
       </c>
       <c r="K114" t="n">
-        <v>954</v>
+        <v>179</v>
       </c>
       <c r="L114" t="inlineStr">
         <is>
@@ -7888,7 +7888,7 @@
         </is>
       </c>
       <c r="K115" t="n">
-        <v>955</v>
+        <v>180</v>
       </c>
       <c r="L115" t="inlineStr">
         <is>
@@ -7954,7 +7954,7 @@
         </is>
       </c>
       <c r="K116" t="n">
-        <v>956</v>
+        <v>181</v>
       </c>
       <c r="L116" t="inlineStr">
         <is>
@@ -8022,7 +8022,7 @@
         </is>
       </c>
       <c r="K117" t="n">
-        <v>957</v>
+        <v>182</v>
       </c>
       <c r="L117" t="inlineStr">
         <is>
@@ -8090,7 +8090,7 @@
         </is>
       </c>
       <c r="K118" t="n">
-        <v>625</v>
+        <v>156</v>
       </c>
       <c r="L118" t="inlineStr">
         <is>
@@ -8158,7 +8158,7 @@
         </is>
       </c>
       <c r="K119" t="n">
-        <v>958</v>
+        <v>183</v>
       </c>
       <c r="L119" t="inlineStr">
         <is>
@@ -8222,7 +8222,7 @@
         </is>
       </c>
       <c r="K120" t="n">
-        <v>959</v>
+        <v>184</v>
       </c>
       <c r="L120" t="inlineStr">
         <is>
@@ -8282,7 +8282,7 @@
         </is>
       </c>
       <c r="K121" t="n">
-        <v>960</v>
+        <v>185</v>
       </c>
       <c r="L121" t="inlineStr">
         <is>
@@ -8346,7 +8346,7 @@
         </is>
       </c>
       <c r="K122" t="n">
-        <v>961</v>
+        <v>186</v>
       </c>
       <c r="L122" t="inlineStr">
         <is>
@@ -8406,7 +8406,7 @@
         </is>
       </c>
       <c r="K123" t="n">
-        <v>962</v>
+        <v>187</v>
       </c>
       <c r="L123" t="inlineStr">
         <is>
@@ -8474,7 +8474,7 @@
         </is>
       </c>
       <c r="K124" t="n">
-        <v>963</v>
+        <v>188</v>
       </c>
       <c r="L124" t="inlineStr">
         <is>
@@ -8538,7 +8538,7 @@
         </is>
       </c>
       <c r="K125" t="n">
-        <v>964</v>
+        <v>189</v>
       </c>
       <c r="L125" t="inlineStr">
         <is>
@@ -8602,7 +8602,7 @@
         </is>
       </c>
       <c r="K126" t="n">
-        <v>965</v>
+        <v>190</v>
       </c>
       <c r="L126" t="inlineStr">
         <is>
@@ -8668,7 +8668,7 @@
         </is>
       </c>
       <c r="K127" t="n">
-        <v>966</v>
+        <v>191</v>
       </c>
       <c r="L127" t="inlineStr">
         <is>
@@ -8728,7 +8728,7 @@
         </is>
       </c>
       <c r="K128" t="n">
-        <v>967</v>
+        <v>192</v>
       </c>
       <c r="L128" t="inlineStr">
         <is>
@@ -8796,7 +8796,7 @@
         </is>
       </c>
       <c r="K129" t="n">
-        <v>968</v>
+        <v>193</v>
       </c>
       <c r="L129" t="inlineStr">
         <is>
@@ -8864,7 +8864,7 @@
         </is>
       </c>
       <c r="K130" t="n">
-        <v>969</v>
+        <v>194</v>
       </c>
       <c r="L130" t="inlineStr">
         <is>
@@ -8928,7 +8928,7 @@
         </is>
       </c>
       <c r="K131" t="n">
-        <v>970</v>
+        <v>195</v>
       </c>
       <c r="L131" t="inlineStr">
         <is>
@@ -8992,7 +8992,7 @@
         </is>
       </c>
       <c r="K132" t="n">
-        <v>971</v>
+        <v>196</v>
       </c>
       <c r="L132" t="inlineStr">
         <is>
@@ -9052,7 +9052,7 @@
         </is>
       </c>
       <c r="K133" t="n">
-        <v>972</v>
+        <v>197</v>
       </c>
       <c r="L133" t="inlineStr">
         <is>
@@ -9112,7 +9112,7 @@
         </is>
       </c>
       <c r="K134" t="n">
-        <v>973</v>
+        <v>198</v>
       </c>
       <c r="L134" t="inlineStr">
         <is>
@@ -9180,7 +9180,7 @@
         </is>
       </c>
       <c r="K135" t="n">
-        <v>974</v>
+        <v>199</v>
       </c>
       <c r="L135" t="inlineStr">
         <is>
@@ -9250,7 +9250,7 @@
         </is>
       </c>
       <c r="K136" t="n">
-        <v>975</v>
+        <v>200</v>
       </c>
       <c r="L136" t="inlineStr">
         <is>
@@ -9314,7 +9314,7 @@
         </is>
       </c>
       <c r="K137" t="n">
-        <v>976</v>
+        <v>201</v>
       </c>
       <c r="L137" t="inlineStr">
         <is>
@@ -9378,7 +9378,7 @@
         </is>
       </c>
       <c r="K138" t="n">
-        <v>977</v>
+        <v>202</v>
       </c>
       <c r="L138" t="inlineStr">
         <is>
@@ -9444,7 +9444,7 @@
         </is>
       </c>
       <c r="K139" t="n">
-        <v>978</v>
+        <v>203</v>
       </c>
       <c r="L139" t="inlineStr">
         <is>
@@ -9512,7 +9512,7 @@
         </is>
       </c>
       <c r="K140" t="n">
-        <v>979</v>
+        <v>204</v>
       </c>
       <c r="L140" t="inlineStr">
         <is>
@@ -9576,7 +9576,7 @@
         </is>
       </c>
       <c r="K141" t="n">
-        <v>674</v>
+        <v>205</v>
       </c>
       <c r="L141" t="inlineStr">
         <is>
@@ -9644,7 +9644,7 @@
         </is>
       </c>
       <c r="K142" t="n">
-        <v>980</v>
+        <v>206</v>
       </c>
       <c r="L142" t="inlineStr">
         <is>
@@ -9708,7 +9708,7 @@
         </is>
       </c>
       <c r="K143" t="n">
-        <v>981</v>
+        <v>207</v>
       </c>
       <c r="L143" t="inlineStr">
         <is>
@@ -9768,7 +9768,7 @@
         </is>
       </c>
       <c r="K144" t="n">
-        <v>982</v>
+        <v>208</v>
       </c>
       <c r="L144" t="inlineStr">
         <is>
@@ -9832,7 +9832,7 @@
         </is>
       </c>
       <c r="K145" t="n">
-        <v>983</v>
+        <v>209</v>
       </c>
       <c r="L145" t="inlineStr">
         <is>
@@ -9892,7 +9892,7 @@
         </is>
       </c>
       <c r="K146" t="n">
-        <v>984</v>
+        <v>210</v>
       </c>
       <c r="L146" t="inlineStr">
         <is>
@@ -9960,7 +9960,7 @@
         </is>
       </c>
       <c r="K147" t="n">
-        <v>985</v>
+        <v>211</v>
       </c>
       <c r="L147" t="inlineStr">
         <is>
@@ -10028,7 +10028,7 @@
         </is>
       </c>
       <c r="K148" t="n">
-        <v>986</v>
+        <v>212</v>
       </c>
       <c r="L148" t="inlineStr">
         <is>
@@ -10092,7 +10092,7 @@
         </is>
       </c>
       <c r="K149" t="n">
-        <v>987</v>
+        <v>213</v>
       </c>
       <c r="L149" t="inlineStr">
         <is>
@@ -10158,7 +10158,7 @@
         </is>
       </c>
       <c r="K150" t="n">
-        <v>988</v>
+        <v>214</v>
       </c>
       <c r="L150" t="inlineStr">
         <is>
@@ -10228,7 +10228,7 @@
         </is>
       </c>
       <c r="K151" t="n">
-        <v>989</v>
+        <v>215</v>
       </c>
       <c r="L151" t="inlineStr">
         <is>
@@ -10292,7 +10292,7 @@
         </is>
       </c>
       <c r="K152" t="n">
-        <v>674</v>
+        <v>205</v>
       </c>
       <c r="L152" t="inlineStr">
         <is>
@@ -10360,7 +10360,7 @@
         </is>
       </c>
       <c r="K153" t="n">
-        <v>990</v>
+        <v>216</v>
       </c>
       <c r="L153" t="inlineStr">
         <is>
@@ -10424,7 +10424,7 @@
         </is>
       </c>
       <c r="K154" t="n">
-        <v>991</v>
+        <v>217</v>
       </c>
       <c r="L154" t="inlineStr">
         <is>
@@ -10484,7 +10484,7 @@
         </is>
       </c>
       <c r="K155" t="n">
-        <v>992</v>
+        <v>218</v>
       </c>
       <c r="L155" t="inlineStr">
         <is>
@@ -10548,7 +10548,7 @@
         </is>
       </c>
       <c r="K156" t="n">
-        <v>993</v>
+        <v>219</v>
       </c>
       <c r="L156" t="inlineStr">
         <is>
@@ -10608,7 +10608,7 @@
         </is>
       </c>
       <c r="K157" t="n">
-        <v>994</v>
+        <v>220</v>
       </c>
       <c r="L157" t="inlineStr">
         <is>
@@ -10676,7 +10676,7 @@
         </is>
       </c>
       <c r="K158" t="n">
-        <v>995</v>
+        <v>221</v>
       </c>
       <c r="L158" t="inlineStr">
         <is>
@@ -10744,7 +10744,7 @@
         </is>
       </c>
       <c r="K159" t="n">
-        <v>996</v>
+        <v>222</v>
       </c>
       <c r="L159" t="inlineStr">
         <is>
@@ -10808,7 +10808,7 @@
         </is>
       </c>
       <c r="K160" t="n">
-        <v>997</v>
+        <v>223</v>
       </c>
       <c r="L160" t="inlineStr">
         <is>
@@ -10874,7 +10874,7 @@
         </is>
       </c>
       <c r="K161" t="n">
-        <v>998</v>
+        <v>224</v>
       </c>
       <c r="L161" t="inlineStr">
         <is>
@@ -10938,7 +10938,7 @@
         </is>
       </c>
       <c r="K162" t="n">
-        <v>674</v>
+        <v>205</v>
       </c>
       <c r="L162" t="inlineStr">
         <is>
@@ -11006,7 +11006,7 @@
         </is>
       </c>
       <c r="K163" t="n">
-        <v>999</v>
+        <v>225</v>
       </c>
       <c r="L163" t="inlineStr">
         <is>
@@ -11070,7 +11070,7 @@
         </is>
       </c>
       <c r="K164" t="n">
-        <v>1000</v>
+        <v>226</v>
       </c>
       <c r="L164" t="inlineStr">
         <is>
@@ -11130,7 +11130,7 @@
         </is>
       </c>
       <c r="K165" t="n">
-        <v>1001</v>
+        <v>227</v>
       </c>
       <c r="L165" t="inlineStr">
         <is>
@@ -11194,7 +11194,7 @@
         </is>
       </c>
       <c r="K166" t="n">
-        <v>1002</v>
+        <v>228</v>
       </c>
       <c r="L166" t="inlineStr">
         <is>
@@ -11254,7 +11254,7 @@
         </is>
       </c>
       <c r="K167" t="n">
-        <v>1003</v>
+        <v>229</v>
       </c>
       <c r="L167" t="inlineStr">
         <is>
@@ -11322,7 +11322,7 @@
         </is>
       </c>
       <c r="K168" t="n">
-        <v>1004</v>
+        <v>230</v>
       </c>
       <c r="L168" t="inlineStr">
         <is>
@@ -11388,7 +11388,7 @@
         </is>
       </c>
       <c r="K169" t="n">
-        <v>1005</v>
+        <v>231</v>
       </c>
       <c r="L169" t="inlineStr">
         <is>
@@ -11458,7 +11458,7 @@
         </is>
       </c>
       <c r="K170" t="n">
-        <v>1006</v>
+        <v>232</v>
       </c>
       <c r="L170" t="inlineStr">
         <is>
@@ -11522,7 +11522,7 @@
         </is>
       </c>
       <c r="K171" t="n">
-        <v>674</v>
+        <v>205</v>
       </c>
       <c r="L171" t="inlineStr">
         <is>
@@ -11590,7 +11590,7 @@
         </is>
       </c>
       <c r="K172" t="n">
-        <v>1007</v>
+        <v>233</v>
       </c>
       <c r="L172" t="inlineStr">
         <is>
@@ -11654,7 +11654,7 @@
         </is>
       </c>
       <c r="K173" t="n">
-        <v>1008</v>
+        <v>234</v>
       </c>
       <c r="L173" t="inlineStr">
         <is>
@@ -11718,7 +11718,7 @@
         </is>
       </c>
       <c r="K174" t="n">
-        <v>1009</v>
+        <v>235</v>
       </c>
       <c r="L174" t="inlineStr">
         <is>
@@ -11786,7 +11786,7 @@
         </is>
       </c>
       <c r="K175" t="n">
-        <v>1010</v>
+        <v>236</v>
       </c>
       <c r="L175" t="inlineStr">
         <is>
@@ -11854,7 +11854,7 @@
         </is>
       </c>
       <c r="K176" t="n">
-        <v>1011</v>
+        <v>237</v>
       </c>
       <c r="L176" t="inlineStr">
         <is>
@@ -11918,7 +11918,7 @@
         </is>
       </c>
       <c r="K177" t="n">
-        <v>1012</v>
+        <v>238</v>
       </c>
       <c r="L177" t="inlineStr">
         <is>
@@ -11984,7 +11984,7 @@
         </is>
       </c>
       <c r="K178" t="n">
-        <v>1013</v>
+        <v>239</v>
       </c>
       <c r="L178" t="inlineStr">
         <is>
@@ -12048,7 +12048,7 @@
         </is>
       </c>
       <c r="K179" t="n">
-        <v>1014</v>
+        <v>240</v>
       </c>
       <c r="L179" t="inlineStr">
         <is>
@@ -12116,7 +12116,7 @@
         </is>
       </c>
       <c r="K180" t="n">
-        <v>1015</v>
+        <v>241</v>
       </c>
       <c r="L180" t="inlineStr">
         <is>
@@ -12184,7 +12184,7 @@
         </is>
       </c>
       <c r="K181" t="n">
-        <v>1016</v>
+        <v>242</v>
       </c>
       <c r="L181" t="inlineStr">
         <is>
@@ -12248,7 +12248,7 @@
         </is>
       </c>
       <c r="K182" t="n">
-        <v>1017</v>
+        <v>243</v>
       </c>
       <c r="L182" t="inlineStr">
         <is>
@@ -12312,7 +12312,7 @@
         </is>
       </c>
       <c r="K183" t="n">
-        <v>1018</v>
+        <v>244</v>
       </c>
       <c r="L183" t="inlineStr">
         <is>
@@ -12376,7 +12376,7 @@
         </is>
       </c>
       <c r="K184" t="n">
-        <v>1019</v>
+        <v>245</v>
       </c>
       <c r="L184" t="inlineStr">
         <is>
@@ -12440,7 +12440,7 @@
         </is>
       </c>
       <c r="K185" t="n">
-        <v>1020</v>
+        <v>246</v>
       </c>
       <c r="L185" t="inlineStr">
         <is>
@@ -12510,7 +12510,7 @@
         </is>
       </c>
       <c r="K186" t="n">
-        <v>1021</v>
+        <v>247</v>
       </c>
       <c r="L186" t="inlineStr">
         <is>
@@ -12574,7 +12574,7 @@
         </is>
       </c>
       <c r="K187" t="n">
-        <v>1022</v>
+        <v>248</v>
       </c>
       <c r="L187" t="inlineStr">
         <is>
@@ -12638,7 +12638,7 @@
         </is>
       </c>
       <c r="K188" t="n">
-        <v>1023</v>
+        <v>249</v>
       </c>
       <c r="L188" t="inlineStr">
         <is>
@@ -12704,7 +12704,7 @@
         </is>
       </c>
       <c r="K189" t="n">
-        <v>1024</v>
+        <v>250</v>
       </c>
       <c r="L189" t="inlineStr">
         <is>
@@ -12772,7 +12772,7 @@
         </is>
       </c>
       <c r="K190" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L190" t="inlineStr">
         <is>
@@ -12838,7 +12838,7 @@
         </is>
       </c>
       <c r="K191" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L191" t="inlineStr">
         <is>
@@ -12900,7 +12900,7 @@
         </is>
       </c>
       <c r="K192" t="n">
-        <v>1025</v>
+        <v>253</v>
       </c>
       <c r="L192" t="inlineStr">
         <is>
@@ -12968,7 +12968,7 @@
         </is>
       </c>
       <c r="K193" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L193" t="inlineStr">
         <is>
@@ -13034,7 +13034,7 @@
         </is>
       </c>
       <c r="K194" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L194" t="inlineStr">
         <is>
@@ -13096,7 +13096,7 @@
         </is>
       </c>
       <c r="K195" t="n">
-        <v>1026</v>
+        <v>254</v>
       </c>
       <c r="L195" t="inlineStr">
         <is>
@@ -13162,7 +13162,7 @@
         </is>
       </c>
       <c r="K196" t="n">
-        <v>1027</v>
+        <v>255</v>
       </c>
       <c r="L196" t="inlineStr">
         <is>
@@ -13230,7 +13230,7 @@
         </is>
       </c>
       <c r="K197" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L197" t="inlineStr">
         <is>
@@ -13296,7 +13296,7 @@
         </is>
       </c>
       <c r="K198" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L198" t="inlineStr">
         <is>
@@ -13358,7 +13358,7 @@
         </is>
       </c>
       <c r="K199" t="n">
-        <v>1028</v>
+        <v>256</v>
       </c>
       <c r="L199" t="inlineStr">
         <is>
@@ -13422,7 +13422,7 @@
         </is>
       </c>
       <c r="K200" t="n">
-        <v>1029</v>
+        <v>257</v>
       </c>
       <c r="L200" t="inlineStr">
         <is>
@@ -13486,7 +13486,7 @@
         </is>
       </c>
       <c r="K201" t="n">
-        <v>1030</v>
+        <v>258</v>
       </c>
       <c r="L201" t="inlineStr">
         <is>
@@ -13550,7 +13550,7 @@
         </is>
       </c>
       <c r="K202" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L202" t="inlineStr">
         <is>
@@ -13616,7 +13616,7 @@
         </is>
       </c>
       <c r="K203" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L203" t="inlineStr">
         <is>
@@ -13678,7 +13678,7 @@
         </is>
       </c>
       <c r="K204" t="n">
-        <v>1031</v>
+        <v>259</v>
       </c>
       <c r="L204" t="inlineStr">
         <is>
@@ -13742,7 +13742,7 @@
         </is>
       </c>
       <c r="K205" t="n">
-        <v>1032</v>
+        <v>260</v>
       </c>
       <c r="L205" t="inlineStr">
         <is>
@@ -13808,7 +13808,7 @@
         </is>
       </c>
       <c r="K206" t="n">
-        <v>1033</v>
+        <v>261</v>
       </c>
       <c r="L206" t="inlineStr">
         <is>
@@ -13876,7 +13876,7 @@
         </is>
       </c>
       <c r="K207" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L207" t="inlineStr">
         <is>
@@ -13942,7 +13942,7 @@
         </is>
       </c>
       <c r="K208" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L208" t="inlineStr">
         <is>
@@ -14004,7 +14004,7 @@
         </is>
       </c>
       <c r="K209" t="n">
-        <v>1034</v>
+        <v>262</v>
       </c>
       <c r="L209" t="inlineStr">
         <is>
@@ -14068,7 +14068,7 @@
         </is>
       </c>
       <c r="K210" t="n">
-        <v>1035</v>
+        <v>263</v>
       </c>
       <c r="L210" t="inlineStr">
         <is>
@@ -14136,7 +14136,7 @@
         </is>
       </c>
       <c r="K211" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L211" t="inlineStr">
         <is>
@@ -14202,7 +14202,7 @@
         </is>
       </c>
       <c r="K212" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L212" t="inlineStr">
         <is>
@@ -14264,7 +14264,7 @@
         </is>
       </c>
       <c r="K213" t="n">
-        <v>1036</v>
+        <v>264</v>
       </c>
       <c r="L213" t="inlineStr">
         <is>
@@ -14330,7 +14330,7 @@
         </is>
       </c>
       <c r="K214" t="n">
-        <v>1037</v>
+        <v>265</v>
       </c>
       <c r="L214" t="inlineStr">
         <is>
@@ -14398,7 +14398,7 @@
         </is>
       </c>
       <c r="K215" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L215" t="inlineStr">
         <is>
@@ -14464,7 +14464,7 @@
         </is>
       </c>
       <c r="K216" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L216" t="inlineStr">
         <is>
@@ -14526,7 +14526,7 @@
         </is>
       </c>
       <c r="K217" t="n">
-        <v>1038</v>
+        <v>266</v>
       </c>
       <c r="L217" t="inlineStr">
         <is>
@@ -14594,7 +14594,7 @@
         </is>
       </c>
       <c r="K218" t="n">
-        <v>720</v>
+        <v>251</v>
       </c>
       <c r="L218" t="inlineStr">
         <is>
@@ -14656,7 +14656,7 @@
         </is>
       </c>
       <c r="K219" t="n">
-        <v>1039</v>
+        <v>267</v>
       </c>
       <c r="L219" t="inlineStr">
         <is>
@@ -14720,7 +14720,7 @@
         </is>
       </c>
       <c r="K220" t="n">
-        <v>1040</v>
+        <v>268</v>
       </c>
       <c r="L220" t="inlineStr">
         <is>
@@ -14784,7 +14784,7 @@
         </is>
       </c>
       <c r="K221" t="n">
-        <v>1041</v>
+        <v>269</v>
       </c>
       <c r="L221" t="inlineStr">
         <is>
@@ -14848,7 +14848,7 @@
         </is>
       </c>
       <c r="K222" t="n">
-        <v>1042</v>
+        <v>270</v>
       </c>
       <c r="L222" t="inlineStr">
         <is>
@@ -14912,7 +14912,7 @@
         </is>
       </c>
       <c r="K223" t="n">
-        <v>1043</v>
+        <v>271</v>
       </c>
       <c r="L223" t="inlineStr">
         <is>
@@ -14978,7 +14978,7 @@
         </is>
       </c>
       <c r="K224" t="n">
-        <v>1044</v>
+        <v>272</v>
       </c>
       <c r="L224" t="inlineStr">
         <is>
@@ -15050,7 +15050,7 @@
         </is>
       </c>
       <c r="K225" t="n">
-        <v>721</v>
+        <v>252</v>
       </c>
       <c r="L225" t="inlineStr">
         <is>
@@ -15116,7 +15116,7 @@
         </is>
       </c>
       <c r="K226" t="n">
-        <v>1045</v>
+        <v>273</v>
       </c>
       <c r="L226" t="inlineStr">
         <is>
@@ -15180,7 +15180,7 @@
         </is>
       </c>
       <c r="K227" t="n">
-        <v>1046</v>
+        <v>274</v>
       </c>
       <c r="L227" t="inlineStr">
         <is>
@@ -15248,7 +15248,7 @@
         </is>
       </c>
       <c r="K228" t="n">
-        <v>1047</v>
+        <v>275</v>
       </c>
       <c r="L228" t="inlineStr">
         <is>
@@ -15312,7 +15312,7 @@
         </is>
       </c>
       <c r="K229" t="n">
-        <v>1048</v>
+        <v>276</v>
       </c>
       <c r="L229" t="inlineStr">
         <is>
@@ -15380,7 +15380,7 @@
         </is>
       </c>
       <c r="K230" t="n">
-        <v>1049</v>
+        <v>277</v>
       </c>
       <c r="L230" t="inlineStr">
         <is>
@@ -15446,7 +15446,7 @@
         </is>
       </c>
       <c r="K231" t="n">
-        <v>1050</v>
+        <v>278</v>
       </c>
       <c r="L231" t="inlineStr">
         <is>
@@ -15516,7 +15516,7 @@
         </is>
       </c>
       <c r="K232" t="n">
-        <v>1051</v>
+        <v>279</v>
       </c>
       <c r="L232" t="inlineStr">
         <is>
@@ -15584,7 +15584,7 @@
         </is>
       </c>
       <c r="K233" t="n">
-        <v>1052</v>
+        <v>280</v>
       </c>
       <c r="L233" t="inlineStr">
         <is>
@@ -15648,7 +15648,7 @@
         </is>
       </c>
       <c r="K234" t="n">
-        <v>1053</v>
+        <v>281</v>
       </c>
       <c r="L234" t="inlineStr">
         <is>
@@ -15712,7 +15712,7 @@
         </is>
       </c>
       <c r="K235" t="n">
-        <v>1054</v>
+        <v>282</v>
       </c>
       <c r="L235" t="inlineStr">
         <is>
@@ -15780,7 +15780,7 @@
         </is>
       </c>
       <c r="K236" t="n">
-        <v>1055</v>
+        <v>283</v>
       </c>
       <c r="L236" t="inlineStr">
         <is>
@@ -15848,7 +15848,7 @@
         </is>
       </c>
       <c r="K237" t="n">
-        <v>1056</v>
+        <v>284</v>
       </c>
       <c r="L237" t="inlineStr">
         <is>
@@ -15912,7 +15912,7 @@
         </is>
       </c>
       <c r="K238" t="n">
-        <v>1057</v>
+        <v>285</v>
       </c>
       <c r="L238" t="inlineStr">
         <is>
@@ -15978,7 +15978,7 @@
         </is>
       </c>
       <c r="K239" t="n">
-        <v>1058</v>
+        <v>286</v>
       </c>
       <c r="L239" t="inlineStr">
         <is>
@@ -16042,7 +16042,7 @@
         </is>
       </c>
       <c r="K240" t="n">
-        <v>1059</v>
+        <v>287</v>
       </c>
       <c r="L240" t="inlineStr">
         <is>
@@ -16106,7 +16106,7 @@
         </is>
       </c>
       <c r="K241" t="n">
-        <v>1060</v>
+        <v>288</v>
       </c>
       <c r="L241" t="inlineStr">
         <is>
@@ -16174,7 +16174,7 @@
         </is>
       </c>
       <c r="K242" t="n">
-        <v>1061</v>
+        <v>289</v>
       </c>
       <c r="L242" t="inlineStr">
         <is>
@@ -16238,7 +16238,7 @@
         </is>
       </c>
       <c r="K243" t="n">
-        <v>1062</v>
+        <v>290</v>
       </c>
       <c r="L243" t="inlineStr">
         <is>
@@ -16302,7 +16302,7 @@
         </is>
       </c>
       <c r="K244" t="n">
-        <v>1063</v>
+        <v>291</v>
       </c>
       <c r="L244" t="inlineStr">
         <is>
@@ -16366,7 +16366,7 @@
         </is>
       </c>
       <c r="K245" t="n">
-        <v>1064</v>
+        <v>292</v>
       </c>
       <c r="L245" t="inlineStr">
         <is>
@@ -16430,7 +16430,7 @@
         </is>
       </c>
       <c r="K246" t="n">
-        <v>1065</v>
+        <v>293</v>
       </c>
       <c r="L246" t="inlineStr">
         <is>
@@ -16500,7 +16500,7 @@
         </is>
       </c>
       <c r="K247" t="n">
-        <v>1066</v>
+        <v>294</v>
       </c>
       <c r="L247" t="inlineStr">
         <is>
@@ -16564,7 +16564,7 @@
         </is>
       </c>
       <c r="K248" t="n">
-        <v>1067</v>
+        <v>295</v>
       </c>
       <c r="L248" t="inlineStr">
         <is>
@@ -16628,7 +16628,7 @@
         </is>
       </c>
       <c r="K249" t="n">
-        <v>1068</v>
+        <v>296</v>
       </c>
       <c r="L249" t="inlineStr">
         <is>
@@ -16694,7 +16694,7 @@
         </is>
       </c>
       <c r="K250" t="n">
-        <v>1069</v>
+        <v>297</v>
       </c>
       <c r="L250" t="inlineStr">
         <is>
@@ -16754,7 +16754,7 @@
         </is>
       </c>
       <c r="K251" t="n">
-        <v>1070</v>
+        <v>298</v>
       </c>
       <c r="L251" t="inlineStr">
         <is>
@@ -16814,7 +16814,7 @@
         </is>
       </c>
       <c r="K252" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L252" t="inlineStr">
         <is>
@@ -16874,7 +16874,7 @@
         </is>
       </c>
       <c r="K253" t="n">
-        <v>1071</v>
+        <v>300</v>
       </c>
       <c r="L253" t="inlineStr">
         <is>
@@ -16934,7 +16934,7 @@
         </is>
       </c>
       <c r="K254" t="n">
-        <v>1072</v>
+        <v>301</v>
       </c>
       <c r="L254" t="inlineStr">
         <is>
@@ -16994,7 +16994,7 @@
         </is>
       </c>
       <c r="K255" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L255" t="inlineStr">
         <is>
@@ -17054,7 +17054,7 @@
         </is>
       </c>
       <c r="K256" t="n">
-        <v>1073</v>
+        <v>302</v>
       </c>
       <c r="L256" t="inlineStr">
         <is>
@@ -17114,7 +17114,7 @@
         </is>
       </c>
       <c r="K257" t="n">
-        <v>1074</v>
+        <v>303</v>
       </c>
       <c r="L257" t="inlineStr">
         <is>
@@ -17174,7 +17174,7 @@
         </is>
       </c>
       <c r="K258" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L258" t="inlineStr">
         <is>
@@ -17234,7 +17234,7 @@
         </is>
       </c>
       <c r="K259" t="n">
-        <v>1075</v>
+        <v>304</v>
       </c>
       <c r="L259" t="inlineStr">
         <is>
@@ -17294,7 +17294,7 @@
         </is>
       </c>
       <c r="K260" t="n">
-        <v>1076</v>
+        <v>305</v>
       </c>
       <c r="L260" t="inlineStr">
         <is>
@@ -17354,7 +17354,7 @@
         </is>
       </c>
       <c r="K261" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L261" t="inlineStr">
         <is>
@@ -17414,7 +17414,7 @@
         </is>
       </c>
       <c r="K262" t="n">
-        <v>1077</v>
+        <v>306</v>
       </c>
       <c r="L262" t="inlineStr">
         <is>
@@ -17474,7 +17474,7 @@
         </is>
       </c>
       <c r="K263" t="n">
-        <v>1078</v>
+        <v>307</v>
       </c>
       <c r="L263" t="inlineStr">
         <is>
@@ -17534,7 +17534,7 @@
         </is>
       </c>
       <c r="K264" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L264" t="inlineStr">
         <is>
@@ -17594,7 +17594,7 @@
         </is>
       </c>
       <c r="K265" t="n">
-        <v>1079</v>
+        <v>308</v>
       </c>
       <c r="L265" t="inlineStr">
         <is>
@@ -17654,7 +17654,7 @@
         </is>
       </c>
       <c r="K266" t="n">
-        <v>1080</v>
+        <v>309</v>
       </c>
       <c r="L266" t="inlineStr">
         <is>
@@ -17714,7 +17714,7 @@
         </is>
       </c>
       <c r="K267" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L267" t="inlineStr">
         <is>
@@ -17774,7 +17774,7 @@
         </is>
       </c>
       <c r="K268" t="n">
-        <v>1081</v>
+        <v>310</v>
       </c>
       <c r="L268" t="inlineStr">
         <is>
@@ -17834,7 +17834,7 @@
         </is>
       </c>
       <c r="K269" t="n">
-        <v>1082</v>
+        <v>311</v>
       </c>
       <c r="L269" t="inlineStr">
         <is>
@@ -17894,7 +17894,7 @@
         </is>
       </c>
       <c r="K270" t="n">
-        <v>1083</v>
+        <v>312</v>
       </c>
       <c r="L270" t="inlineStr">
         <is>
@@ -17952,7 +17952,7 @@
         </is>
       </c>
       <c r="K271" t="n">
-        <v>768</v>
+        <v>299</v>
       </c>
       <c r="L271" t="inlineStr">
         <is>
@@ -18012,7 +18012,7 @@
         </is>
       </c>
       <c r="K272" t="n">
-        <v>782</v>
+        <v>313</v>
       </c>
       <c r="L272" t="inlineStr">
         <is>
@@ -18072,7 +18072,7 @@
         </is>
       </c>
       <c r="K273" t="n">
-        <v>1084</v>
+        <v>314</v>
       </c>
       <c r="L273" t="inlineStr">
         <is>
@@ -18132,7 +18132,7 @@
         </is>
       </c>
       <c r="K274" t="n">
-        <v>1085</v>
+        <v>315</v>
       </c>
       <c r="L274" t="inlineStr">
         <is>
@@ -18192,7 +18192,7 @@
         </is>
       </c>
       <c r="K275" t="n">
-        <v>1086</v>
+        <v>316</v>
       </c>
       <c r="L275" t="inlineStr">
         <is>
@@ -18252,7 +18252,7 @@
         </is>
       </c>
       <c r="K276" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L276" t="inlineStr">
         <is>
@@ -18312,7 +18312,7 @@
         </is>
       </c>
       <c r="K277" t="n">
-        <v>1087</v>
+        <v>318</v>
       </c>
       <c r="L277" t="inlineStr">
         <is>
@@ -18374,7 +18374,7 @@
         </is>
       </c>
       <c r="K278" t="n">
-        <v>782</v>
+        <v>313</v>
       </c>
       <c r="L278" t="inlineStr">
         <is>
@@ -18434,7 +18434,7 @@
         </is>
       </c>
       <c r="K279" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L279" t="inlineStr">
         <is>
@@ -18494,7 +18494,7 @@
         </is>
       </c>
       <c r="K280" t="n">
-        <v>1088</v>
+        <v>319</v>
       </c>
       <c r="L280" t="inlineStr">
         <is>
@@ -18550,7 +18550,7 @@
         </is>
       </c>
       <c r="K281" t="n">
-        <v>1089</v>
+        <v>320</v>
       </c>
       <c r="L281" t="inlineStr">
         <is>
@@ -18610,7 +18610,7 @@
         </is>
       </c>
       <c r="K282" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L282" t="inlineStr">
         <is>
@@ -18670,7 +18670,7 @@
         </is>
       </c>
       <c r="K283" t="n">
-        <v>1090</v>
+        <v>321</v>
       </c>
       <c r="L283" t="inlineStr">
         <is>
@@ -18730,7 +18730,7 @@
         </is>
       </c>
       <c r="K284" t="n">
-        <v>1091</v>
+        <v>322</v>
       </c>
       <c r="L284" t="inlineStr">
         <is>
@@ -18790,7 +18790,7 @@
         </is>
       </c>
       <c r="K285" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L285" t="inlineStr">
         <is>
@@ -18850,7 +18850,7 @@
         </is>
       </c>
       <c r="K286" t="n">
-        <v>1092</v>
+        <v>323</v>
       </c>
       <c r="L286" t="inlineStr">
         <is>
@@ -18910,7 +18910,7 @@
         </is>
       </c>
       <c r="K287" t="n">
-        <v>1093</v>
+        <v>324</v>
       </c>
       <c r="L287" t="inlineStr">
         <is>
@@ -18970,7 +18970,7 @@
         </is>
       </c>
       <c r="K288" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L288" t="inlineStr">
         <is>
@@ -19030,7 +19030,7 @@
         </is>
       </c>
       <c r="K289" t="n">
-        <v>1094</v>
+        <v>325</v>
       </c>
       <c r="L289" t="inlineStr">
         <is>
@@ -19090,7 +19090,7 @@
         </is>
       </c>
       <c r="K290" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L290" t="inlineStr">
         <is>
@@ -19150,7 +19150,7 @@
         </is>
       </c>
       <c r="K291" t="n">
-        <v>1095</v>
+        <v>326</v>
       </c>
       <c r="L291" t="inlineStr">
         <is>
@@ -19210,7 +19210,7 @@
         </is>
       </c>
       <c r="K292" t="n">
-        <v>1096</v>
+        <v>327</v>
       </c>
       <c r="L292" t="inlineStr">
         <is>
@@ -19270,7 +19270,7 @@
         </is>
       </c>
       <c r="K293" t="n">
-        <v>1097</v>
+        <v>328</v>
       </c>
       <c r="L293" t="inlineStr">
         <is>
@@ -19332,7 +19332,7 @@
         </is>
       </c>
       <c r="K294" t="n">
-        <v>786</v>
+        <v>317</v>
       </c>
       <c r="L294" t="inlineStr">
         <is>
@@ -19392,7 +19392,7 @@
         </is>
       </c>
       <c r="K295" t="n">
-        <v>1098</v>
+        <v>329</v>
       </c>
       <c r="L295" t="inlineStr">
         <is>
@@ -19448,7 +19448,7 @@
         </is>
       </c>
       <c r="K296" t="n">
-        <v>1099</v>
+        <v>330</v>
       </c>
       <c r="L296" t="inlineStr">
         <is>
@@ -19508,7 +19508,7 @@
         </is>
       </c>
       <c r="K297" t="n">
-        <v>1100</v>
+        <v>331</v>
       </c>
       <c r="L297" t="inlineStr">
         <is>
@@ -19568,7 +19568,7 @@
         </is>
       </c>
       <c r="K298" t="n">
-        <v>1101</v>
+        <v>332</v>
       </c>
       <c r="L298" t="inlineStr">
         <is>
@@ -19628,7 +19628,7 @@
         </is>
       </c>
       <c r="K299" t="n">
-        <v>1102</v>
+        <v>333</v>
       </c>
       <c r="L299" t="inlineStr">
         <is>
@@ -19688,7 +19688,7 @@
         </is>
       </c>
       <c r="K300" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L300" t="inlineStr">
         <is>
@@ -19748,7 +19748,7 @@
         </is>
       </c>
       <c r="K301" t="n">
-        <v>1103</v>
+        <v>335</v>
       </c>
       <c r="L301" t="inlineStr">
         <is>
@@ -19808,7 +19808,7 @@
         </is>
       </c>
       <c r="K302" t="n">
-        <v>1104</v>
+        <v>336</v>
       </c>
       <c r="L302" t="inlineStr">
         <is>
@@ -19868,7 +19868,7 @@
         </is>
       </c>
       <c r="K303" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L303" t="inlineStr">
         <is>
@@ -19928,7 +19928,7 @@
         </is>
       </c>
       <c r="K304" t="n">
-        <v>1105</v>
+        <v>337</v>
       </c>
       <c r="L304" t="inlineStr">
         <is>
@@ -19988,7 +19988,7 @@
         </is>
       </c>
       <c r="K305" t="n">
-        <v>1106</v>
+        <v>338</v>
       </c>
       <c r="L305" t="inlineStr">
         <is>
@@ -20048,7 +20048,7 @@
         </is>
       </c>
       <c r="K306" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L306" t="inlineStr">
         <is>
@@ -20108,7 +20108,7 @@
         </is>
       </c>
       <c r="K307" t="n">
-        <v>1107</v>
+        <v>339</v>
       </c>
       <c r="L307" t="inlineStr">
         <is>
@@ -20168,7 +20168,7 @@
         </is>
       </c>
       <c r="K308" t="n">
-        <v>1108</v>
+        <v>340</v>
       </c>
       <c r="L308" t="inlineStr">
         <is>
@@ -20228,7 +20228,7 @@
         </is>
       </c>
       <c r="K309" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L309" t="inlineStr">
         <is>
@@ -20288,7 +20288,7 @@
         </is>
       </c>
       <c r="K310" t="n">
-        <v>1109</v>
+        <v>341</v>
       </c>
       <c r="L310" t="inlineStr">
         <is>
@@ -20348,7 +20348,7 @@
         </is>
       </c>
       <c r="K311" t="n">
-        <v>1110</v>
+        <v>342</v>
       </c>
       <c r="L311" t="inlineStr">
         <is>
@@ -20408,7 +20408,7 @@
         </is>
       </c>
       <c r="K312" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L312" t="inlineStr">
         <is>
@@ -20468,7 +20468,7 @@
         </is>
       </c>
       <c r="K313" t="n">
-        <v>1111</v>
+        <v>343</v>
       </c>
       <c r="L313" t="inlineStr">
         <is>
@@ -20528,7 +20528,7 @@
         </is>
       </c>
       <c r="K314" t="n">
-        <v>1112</v>
+        <v>344</v>
       </c>
       <c r="L314" t="inlineStr">
         <is>
@@ -20588,7 +20588,7 @@
         </is>
       </c>
       <c r="K315" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L315" t="inlineStr">
         <is>
@@ -20648,7 +20648,7 @@
         </is>
       </c>
       <c r="K316" t="n">
-        <v>1113</v>
+        <v>345</v>
       </c>
       <c r="L316" t="inlineStr">
         <is>
@@ -20708,7 +20708,7 @@
         </is>
       </c>
       <c r="K317" t="n">
-        <v>1114</v>
+        <v>346</v>
       </c>
       <c r="L317" t="inlineStr">
         <is>
@@ -20768,7 +20768,7 @@
         </is>
       </c>
       <c r="K318" t="n">
-        <v>1115</v>
+        <v>347</v>
       </c>
       <c r="L318" t="inlineStr">
         <is>
@@ -20826,7 +20826,7 @@
         </is>
       </c>
       <c r="K319" t="n">
-        <v>803</v>
+        <v>334</v>
       </c>
       <c r="L319" t="inlineStr">
         <is>
@@ -20886,7 +20886,7 @@
         </is>
       </c>
       <c r="K320" t="n">
-        <v>817</v>
+        <v>348</v>
       </c>
       <c r="L320" t="inlineStr">
         <is>
@@ -20942,7 +20942,7 @@
         </is>
       </c>
       <c r="K321" t="n">
-        <v>1116</v>
+        <v>349</v>
       </c>
       <c r="L321" t="inlineStr">
         <is>
@@ -21002,7 +21002,7 @@
         </is>
       </c>
       <c r="K322" t="n">
-        <v>1117</v>
+        <v>350</v>
       </c>
       <c r="L322" t="inlineStr">
         <is>
@@ -21062,7 +21062,7 @@
         </is>
       </c>
       <c r="K323" t="n">
-        <v>1118</v>
+        <v>351</v>
       </c>
       <c r="L323" t="inlineStr">
         <is>
@@ -21122,7 +21122,7 @@
         </is>
       </c>
       <c r="K324" t="n">
-        <v>1119</v>
+        <v>352</v>
       </c>
       <c r="L324" t="inlineStr">
         <is>
@@ -21178,7 +21178,7 @@
         </is>
       </c>
       <c r="K325" t="n">
-        <v>1120</v>
+        <v>353</v>
       </c>
       <c r="L325" t="inlineStr">
         <is>
@@ -21240,7 +21240,7 @@
         </is>
       </c>
       <c r="K326" t="n">
-        <v>817</v>
+        <v>348</v>
       </c>
       <c r="L326" t="inlineStr">
         <is>
@@ -21300,7 +21300,7 @@
         </is>
       </c>
       <c r="K327" t="n">
-        <v>1121</v>
+        <v>354</v>
       </c>
       <c r="L327" t="inlineStr">
         <is>
@@ -21356,7 +21356,7 @@
         </is>
       </c>
       <c r="K328" t="n">
-        <v>1122</v>
+        <v>355</v>
       </c>
       <c r="L328" t="inlineStr">
         <is>
@@ -21416,7 +21416,7 @@
         </is>
       </c>
       <c r="K329" t="n">
-        <v>1123</v>
+        <v>356</v>
       </c>
       <c r="L329" t="inlineStr">
         <is>
@@ -21476,7 +21476,7 @@
         </is>
       </c>
       <c r="K330" t="n">
-        <v>1124</v>
+        <v>357</v>
       </c>
       <c r="L330" t="inlineStr">
         <is>
@@ -21536,7 +21536,7 @@
         </is>
       </c>
       <c r="K331" t="n">
-        <v>1125</v>
+        <v>358</v>
       </c>
       <c r="L331" t="inlineStr">
         <is>
@@ -21596,7 +21596,7 @@
         </is>
       </c>
       <c r="K332" t="n">
-        <v>1126</v>
+        <v>359</v>
       </c>
       <c r="L332" t="inlineStr">
         <is>
@@ -21656,7 +21656,7 @@
         </is>
       </c>
       <c r="K333" t="n">
-        <v>1127</v>
+        <v>360</v>
       </c>
       <c r="L333" t="inlineStr">
         <is>
@@ -21712,7 +21712,7 @@
         </is>
       </c>
       <c r="K334" t="n">
-        <v>1128</v>
+        <v>361</v>
       </c>
       <c r="L334" t="inlineStr">
         <is>
@@ -21768,7 +21768,7 @@
         </is>
       </c>
       <c r="K335" t="n">
-        <v>831</v>
+        <v>362</v>
       </c>
       <c r="L335" t="inlineStr">
         <is>
@@ -21828,7 +21828,7 @@
         </is>
       </c>
       <c r="K336" t="n">
-        <v>1129</v>
+        <v>363</v>
       </c>
       <c r="L336" t="inlineStr">
         <is>
@@ -21888,7 +21888,7 @@
         </is>
       </c>
       <c r="K337" t="n">
-        <v>1130</v>
+        <v>364</v>
       </c>
       <c r="L337" t="inlineStr">
         <is>
@@ -21948,7 +21948,7 @@
         </is>
       </c>
       <c r="K338" t="n">
-        <v>1131</v>
+        <v>365</v>
       </c>
       <c r="L338" t="inlineStr">
         <is>
@@ -22008,7 +22008,7 @@
         </is>
       </c>
       <c r="K339" t="n">
-        <v>1132</v>
+        <v>366</v>
       </c>
       <c r="L339" t="inlineStr">
         <is>
@@ -22070,7 +22070,7 @@
         </is>
       </c>
       <c r="K340" t="n">
-        <v>831</v>
+        <v>362</v>
       </c>
       <c r="L340" t="inlineStr">
         <is>
@@ -22130,7 +22130,7 @@
         </is>
       </c>
       <c r="K341" t="n">
-        <v>1133</v>
+        <v>367</v>
       </c>
       <c r="L341" t="inlineStr">
         <is>
@@ -22190,7 +22190,7 @@
         </is>
       </c>
       <c r="K342" t="n">
-        <v>1134</v>
+        <v>368</v>
       </c>
       <c r="L342" t="inlineStr">
         <is>
@@ -22250,7 +22250,7 @@
         </is>
       </c>
       <c r="K343" t="n">
-        <v>1135</v>
+        <v>369</v>
       </c>
       <c r="L343" t="inlineStr">
         <is>
@@ -22306,7 +22306,7 @@
         </is>
       </c>
       <c r="K344" t="n">
-        <v>1136</v>
+        <v>370</v>
       </c>
       <c r="L344" t="inlineStr">
         <is>
@@ -22366,7 +22366,7 @@
         </is>
       </c>
       <c r="K345" t="n">
-        <v>1137</v>
+        <v>371</v>
       </c>
       <c r="L345" t="inlineStr">
         <is>
@@ -22426,7 +22426,7 @@
         </is>
       </c>
       <c r="K346" t="n">
-        <v>1138</v>
+        <v>372</v>
       </c>
       <c r="L346" t="inlineStr">
         <is>
@@ -22486,7 +22486,7 @@
         </is>
       </c>
       <c r="K347" t="n">
-        <v>1139</v>
+        <v>373</v>
       </c>
       <c r="L347" t="inlineStr">
         <is>
@@ -22546,7 +22546,7 @@
         </is>
       </c>
       <c r="K348" t="n">
-        <v>1140</v>
+        <v>374</v>
       </c>
       <c r="L348" t="inlineStr">
         <is>
@@ -22606,7 +22606,7 @@
         </is>
       </c>
       <c r="K349" t="n">
-        <v>1141</v>
+        <v>375</v>
       </c>
       <c r="L349" t="inlineStr">
         <is>
@@ -22666,7 +22666,7 @@
         </is>
       </c>
       <c r="K350" t="n">
-        <v>1142</v>
+        <v>376</v>
       </c>
       <c r="L350" t="inlineStr">
         <is>
@@ -22726,7 +22726,7 @@
         </is>
       </c>
       <c r="K351" t="n">
-        <v>1143</v>
+        <v>377</v>
       </c>
       <c r="L351" t="inlineStr">
         <is>
@@ -22786,7 +22786,7 @@
         </is>
       </c>
       <c r="K352" t="n">
-        <v>847</v>
+        <v>378</v>
       </c>
       <c r="L352" t="inlineStr">
         <is>
@@ -22846,7 +22846,7 @@
         </is>
       </c>
       <c r="K353" t="n">
-        <v>1144</v>
+        <v>379</v>
       </c>
       <c r="L353" t="inlineStr">
         <is>
@@ -22906,7 +22906,7 @@
         </is>
       </c>
       <c r="K354" t="n">
-        <v>1145</v>
+        <v>380</v>
       </c>
       <c r="L354" t="inlineStr">
         <is>
@@ -22966,7 +22966,7 @@
         </is>
       </c>
       <c r="K355" t="n">
-        <v>1146</v>
+        <v>381</v>
       </c>
       <c r="L355" t="inlineStr">
         <is>
@@ -23026,7 +23026,7 @@
         </is>
       </c>
       <c r="K356" t="n">
-        <v>1147</v>
+        <v>382</v>
       </c>
       <c r="L356" t="inlineStr">
         <is>
@@ -23086,7 +23086,7 @@
         </is>
       </c>
       <c r="K357" t="n">
-        <v>1148</v>
+        <v>383</v>
       </c>
       <c r="L357" t="inlineStr">
         <is>
@@ -23146,7 +23146,7 @@
         </is>
       </c>
       <c r="K358" t="n">
-        <v>847</v>
+        <v>378</v>
       </c>
       <c r="L358" t="inlineStr">
         <is>
@@ -23206,7 +23206,7 @@
         </is>
       </c>
       <c r="K359" t="n">
-        <v>1149</v>
+        <v>384</v>
       </c>
       <c r="L359" t="inlineStr">
         <is>
@@ -23266,7 +23266,7 @@
         </is>
       </c>
       <c r="K360" t="n">
-        <v>1150</v>
+        <v>385</v>
       </c>
       <c r="L360" t="inlineStr">
         <is>
@@ -23326,7 +23326,7 @@
         </is>
       </c>
       <c r="K361" t="n">
-        <v>1151</v>
+        <v>386</v>
       </c>
       <c r="L361" t="inlineStr">
         <is>
@@ -23382,7 +23382,7 @@
         </is>
       </c>
       <c r="K362" t="n">
-        <v>1152</v>
+        <v>387</v>
       </c>
       <c r="L362" t="inlineStr">
         <is>
@@ -23442,7 +23442,7 @@
         </is>
       </c>
       <c r="K363" t="n">
-        <v>1153</v>
+        <v>388</v>
       </c>
       <c r="L363" t="inlineStr">
         <is>
@@ -23502,7 +23502,7 @@
         </is>
       </c>
       <c r="K364" t="n">
-        <v>1154</v>
+        <v>389</v>
       </c>
       <c r="L364" t="inlineStr">
         <is>
@@ -23564,7 +23564,7 @@
         </is>
       </c>
       <c r="K365" t="n">
-        <v>847</v>
+        <v>378</v>
       </c>
       <c r="L365" t="inlineStr">
         <is>
@@ -23624,7 +23624,7 @@
         </is>
       </c>
       <c r="K366" t="n">
-        <v>1155</v>
+        <v>390</v>
       </c>
       <c r="L366" t="inlineStr">
         <is>
@@ -23680,7 +23680,7 @@
         </is>
       </c>
       <c r="K367" t="n">
-        <v>860</v>
+        <v>391</v>
       </c>
       <c r="L367" t="inlineStr">
         <is>
@@ -23740,7 +23740,7 @@
         </is>
       </c>
       <c r="K368" t="n">
-        <v>861</v>
+        <v>392</v>
       </c>
       <c r="L368" t="inlineStr">
         <is>
@@ -23800,7 +23800,7 @@
         </is>
       </c>
       <c r="K369" t="n">
-        <v>862</v>
+        <v>393</v>
       </c>
       <c r="L369" t="inlineStr">
         <is>
@@ -23860,7 +23860,7 @@
         </is>
       </c>
       <c r="K370" t="n">
-        <v>1156</v>
+        <v>394</v>
       </c>
       <c r="L370" t="inlineStr">
         <is>
@@ -23920,7 +23920,7 @@
         </is>
       </c>
       <c r="K371" t="n">
-        <v>1157</v>
+        <v>395</v>
       </c>
       <c r="L371" t="inlineStr">
         <is>
@@ -23980,7 +23980,7 @@
         </is>
       </c>
       <c r="K372" t="n">
-        <v>1158</v>
+        <v>396</v>
       </c>
       <c r="L372" t="inlineStr">
         <is>
@@ -24040,7 +24040,7 @@
         </is>
       </c>
       <c r="K373" t="n">
-        <v>1159</v>
+        <v>397</v>
       </c>
       <c r="L373" t="inlineStr">
         <is>
@@ -24100,7 +24100,7 @@
         </is>
       </c>
       <c r="K374" t="n">
-        <v>1160</v>
+        <v>398</v>
       </c>
       <c r="L374" t="inlineStr">
         <is>
@@ -24162,7 +24162,7 @@
         </is>
       </c>
       <c r="K375" t="n">
-        <v>847</v>
+        <v>378</v>
       </c>
       <c r="L375" t="inlineStr">
         <is>
@@ -24222,7 +24222,7 @@
         </is>
       </c>
       <c r="K376" t="n">
-        <v>1161</v>
+        <v>399</v>
       </c>
       <c r="L376" t="inlineStr">
         <is>
@@ -24280,7 +24280,7 @@
         </is>
       </c>
       <c r="K377" t="n">
-        <v>860</v>
+        <v>391</v>
       </c>
       <c r="L377" t="inlineStr">
         <is>
@@ -24340,7 +24340,7 @@
         </is>
       </c>
       <c r="K378" t="n">
-        <v>869</v>
+        <v>400</v>
       </c>
       <c r="L378" t="inlineStr">
         <is>
@@ -24400,7 +24400,7 @@
         </is>
       </c>
       <c r="K379" t="n">
-        <v>1162</v>
+        <v>401</v>
       </c>
       <c r="L379" t="inlineStr">
         <is>
@@ -24458,7 +24458,7 @@
         </is>
       </c>
       <c r="K380" t="n">
-        <v>862</v>
+        <v>393</v>
       </c>
       <c r="L380" t="inlineStr">
         <is>
@@ -24518,7 +24518,7 @@
         </is>
       </c>
       <c r="K381" t="n">
-        <v>861</v>
+        <v>392</v>
       </c>
       <c r="L381" t="inlineStr">
         <is>
@@ -24578,7 +24578,7 @@
         </is>
       </c>
       <c r="K382" t="n">
-        <v>1163</v>
+        <v>402</v>
       </c>
       <c r="L382" t="inlineStr">
         <is>
@@ -24638,7 +24638,7 @@
         </is>
       </c>
       <c r="K383" t="n">
-        <v>1164</v>
+        <v>403</v>
       </c>
       <c r="L383" t="inlineStr">
         <is>
@@ -24698,7 +24698,7 @@
         </is>
       </c>
       <c r="K384" t="n">
-        <v>1165</v>
+        <v>404</v>
       </c>
       <c r="L384" t="inlineStr">
         <is>
@@ -24758,7 +24758,7 @@
         </is>
       </c>
       <c r="K385" t="n">
-        <v>1166</v>
+        <v>405</v>
       </c>
       <c r="L385" t="inlineStr">
         <is>
@@ -24820,7 +24820,7 @@
         </is>
       </c>
       <c r="K386" t="n">
-        <v>847</v>
+        <v>378</v>
       </c>
       <c r="L386" t="inlineStr">
         <is>
@@ -24880,7 +24880,7 @@
         </is>
       </c>
       <c r="K387" t="n">
-        <v>1167</v>
+        <v>406</v>
       </c>
       <c r="L387" t="inlineStr">
         <is>
@@ -24936,7 +24936,7 @@
         </is>
       </c>
       <c r="K388" t="n">
-        <v>1168</v>
+        <v>407</v>
       </c>
       <c r="L388" t="inlineStr">
         <is>
@@ -24994,7 +24994,7 @@
         </is>
       </c>
       <c r="K389" t="n">
-        <v>869</v>
+        <v>400</v>
       </c>
       <c r="L389" t="inlineStr">
         <is>
@@ -25054,7 +25054,7 @@
         </is>
       </c>
       <c r="K390" t="n">
-        <v>1169</v>
+        <v>408</v>
       </c>
       <c r="L390" t="inlineStr">
         <is>
@@ -25112,7 +25112,7 @@
         </is>
       </c>
       <c r="K391" t="n">
-        <v>861</v>
+        <v>392</v>
       </c>
       <c r="L391" t="inlineStr">
         <is>
@@ -25172,7 +25172,7 @@
         </is>
       </c>
       <c r="K392" t="n">
-        <v>1170</v>
+        <v>409</v>
       </c>
       <c r="L392" t="inlineStr">
         <is>

</xml_diff>